<commit_message>
Refactor test setup and enhance report generation
Moved test fixtures to a new `conftest.py` for cleaner test organization. Added tests for performance report generation and updated dependencies to include `pyarrow` and `openpyxl` for improved functionality. Simplified `_compute` logic in `generate_perf_report.py` by removing redundant directory creation.
</commit_message>
<xml_diff>
--- a/outputs/funds_perf_report.xlsx
+++ b/outputs/funds_perf_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,318 +465,6 @@
         </is>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>2022-08</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Gohen</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>13.28566009764734</v>
-      </c>
-      <c r="D2" t="n">
-        <v>585569.7282415634</v>
-      </c>
-      <c r="E2" t="n">
-        <v>8630204.692416647</v>
-      </c>
-      <c r="F2" t="n">
-        <v>-264954.5912859503</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>2022-09</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Trustmind</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>2.88726404923217</v>
-      </c>
-      <c r="D3" t="n">
-        <v>10620015.04946109</v>
-      </c>
-      <c r="E3" t="n">
-        <v>43758645.49386902</v>
-      </c>
-      <c r="F3" t="n">
-        <v>-2475842.789794324</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>2022-10</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Wallington</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>3.62743153784914</v>
-      </c>
-      <c r="D4" t="n">
-        <v>41969174.17637323</v>
-      </c>
-      <c r="E4" t="n">
-        <v>196905682.1293281</v>
-      </c>
-      <c r="F4" t="n">
-        <v>-2696201.928094937</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>2022-11</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Leeder</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>7.028914070404999</v>
-      </c>
-      <c r="D5" t="n">
-        <v>2292900.69230508</v>
-      </c>
-      <c r="E5" t="n">
-        <v>26801108.0777934</v>
-      </c>
-      <c r="F5" t="n">
-        <v>-8391605.447303778</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>2022-12</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Gohen</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>77.7271359243389</v>
-      </c>
-      <c r="D6" t="n">
-        <v>205432.9423791791</v>
-      </c>
-      <c r="E6" t="n">
-        <v>16104397.4604946</v>
-      </c>
-      <c r="F6" t="n">
-        <v>68749.71752790874</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>2023-01</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Magnum</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>7.368744008398862</v>
-      </c>
-      <c r="D7" t="n">
-        <v>7696183.77063203</v>
-      </c>
-      <c r="E7" t="n">
-        <v>59924748.15551724</v>
-      </c>
-      <c r="F7" t="n">
-        <v>4482643.662496128</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>2023-02</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Applebead</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>12.86993986056393</v>
-      </c>
-      <c r="D8" t="n">
-        <v>9386135.624031307</v>
-      </c>
-      <c r="E8" t="n">
-        <v>129673836.4555226</v>
-      </c>
-      <c r="F8" t="n">
-        <v>511300.1728883917</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>2023-03</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Catalysm</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>11.49391751539593</v>
-      </c>
-      <c r="D9" t="n">
-        <v>193275.2141059854</v>
-      </c>
-      <c r="E9" t="n">
-        <v>2618183.302886812</v>
-      </c>
-      <c r="F9" t="n">
-        <v>-203418.7200761429</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>2023-04</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Gohen</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>829.6124356178589</v>
-      </c>
-      <c r="D10" t="n">
-        <v>4968.622816473871</v>
-      </c>
-      <c r="E10" t="n">
-        <v>3436686.273461192</v>
-      </c>
-      <c r="F10" t="n">
-        <v>690313.6257966359</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>2023-05</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Gohen</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>19.81385261671864</v>
-      </c>
-      <c r="D11" t="n">
-        <v>227211.4984409648</v>
-      </c>
-      <c r="E11" t="n">
-        <v>5217218.028098187</v>
-      </c>
-      <c r="F11" t="n">
-        <v>-488071.3867241474</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>2023-06</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Gohen</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>19.69453756641664</v>
-      </c>
-      <c r="D12" t="n">
-        <v>536075.8121401727</v>
-      </c>
-      <c r="E12" t="n">
-        <v>10912906.70472738</v>
-      </c>
-      <c r="F12" t="n">
-        <v>180934.3280547339</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>2023-07</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Applebead</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>66.01470618098682</v>
-      </c>
-      <c r="D13" t="n">
-        <v>10094131.24441911</v>
-      </c>
-      <c r="E13" t="n">
-        <v>675074648.1844716</v>
-      </c>
-      <c r="F13" t="n">
-        <v>1380591.312594123</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>2023-08</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Applebead</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>9.516932644869431</v>
-      </c>
-      <c r="D14" t="n">
-        <v>5513343.953973653</v>
-      </c>
-      <c r="E14" t="n">
-        <v>60651817.36173481</v>
-      </c>
-      <c r="F14" t="n">
-        <v>-2668350.349795799</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Refactor fund report generation and update tests.
Modified `generate_best_performing_fund_report` to optionally return a DataFrame, enabling more focused testing. Refactored and simplified tests to align with the updated function logic, ensuring improved clarity and maintainability. Updated sample data to better reflect edge cases.
</commit_message>
<xml_diff>
--- a/outputs/funds_perf_report.xlsx
+++ b/outputs/funds_perf_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,30 @@
         </is>
       </c>
     </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>2024-01</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Alpha</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="E2" t="n">
+        <v>1200</v>
+      </c>
+      <c r="F2" t="n">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove unused secret_key attribute from Config class
The secret_key attribute was redundant and is now removed for cleanup. Additionally, unrelated output files have been updated, but no changes were made to their functionality within the code.
</commit_message>
<xml_diff>
--- a/outputs/funds_perf_report.xlsx
+++ b/outputs/funds_perf_report.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,25 +468,313 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>2024-01</t>
+          <t>2022-08</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Alpha</t>
+          <t>Gohen</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0.3</v>
+        <v>13.28566009764734</v>
       </c>
       <c r="D2" t="n">
-        <v>1000</v>
+        <v>585569.7282415634</v>
       </c>
       <c r="E2" t="n">
-        <v>1200</v>
+        <v>8630204.692416647</v>
       </c>
       <c r="F2" t="n">
-        <v>100</v>
+        <v>-264954.5912859503</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>2022-09</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Trustmind</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>2.88726404923217</v>
+      </c>
+      <c r="D3" t="n">
+        <v>10620015.04946109</v>
+      </c>
+      <c r="E3" t="n">
+        <v>43758645.49386902</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-2475842.789794324</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>2022-10</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Wallington</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>3.62743153784914</v>
+      </c>
+      <c r="D4" t="n">
+        <v>41969174.17637323</v>
+      </c>
+      <c r="E4" t="n">
+        <v>196905682.1293281</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-2696201.928094937</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>2022-11</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Leeder</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>7.028914070404999</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2292900.69230508</v>
+      </c>
+      <c r="E5" t="n">
+        <v>26801108.0777934</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-8391605.447303778</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>2022-12</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Gohen</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>77.7271359243389</v>
+      </c>
+      <c r="D6" t="n">
+        <v>205432.9423791791</v>
+      </c>
+      <c r="E6" t="n">
+        <v>16104397.4604946</v>
+      </c>
+      <c r="F6" t="n">
+        <v>68749.71752790874</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>2023-01</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Magnum</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>7.368744008398862</v>
+      </c>
+      <c r="D7" t="n">
+        <v>7696183.77063203</v>
+      </c>
+      <c r="E7" t="n">
+        <v>59924748.15551724</v>
+      </c>
+      <c r="F7" t="n">
+        <v>4482643.662496128</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>2023-02</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Applebead</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>12.86993986056393</v>
+      </c>
+      <c r="D8" t="n">
+        <v>9386135.624031307</v>
+      </c>
+      <c r="E8" t="n">
+        <v>129673836.4555226</v>
+      </c>
+      <c r="F8" t="n">
+        <v>511300.1728883917</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2023-03</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Catalysm</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>11.49391751539593</v>
+      </c>
+      <c r="D9" t="n">
+        <v>193275.2141059854</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2618183.302886812</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-203418.7200761429</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>2023-04</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Gohen</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>829.6124356178589</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4968.622816473871</v>
+      </c>
+      <c r="E10" t="n">
+        <v>3436686.273461192</v>
+      </c>
+      <c r="F10" t="n">
+        <v>690313.6257966359</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>2023-05</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Gohen</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>19.81385261671864</v>
+      </c>
+      <c r="D11" t="n">
+        <v>227211.4984409648</v>
+      </c>
+      <c r="E11" t="n">
+        <v>5217218.028098187</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-488071.3867241474</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>2023-06</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Gohen</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>19.69453756641664</v>
+      </c>
+      <c r="D12" t="n">
+        <v>536075.8121401727</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10912906.70472738</v>
+      </c>
+      <c r="F12" t="n">
+        <v>180934.3280547339</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>2023-07</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Applebead</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>66.01470618098682</v>
+      </c>
+      <c r="D13" t="n">
+        <v>10094131.24441911</v>
+      </c>
+      <c r="E13" t="n">
+        <v>675074648.1844716</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1380591.312594123</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>2023-08</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Applebead</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>9.516932644869431</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5513343.953973653</v>
+      </c>
+      <c r="E14" t="n">
+        <v>60651817.36173481</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-2668350.349795799</v>
       </c>
     </row>
   </sheetData>

</xml_diff>